<commit_message>
Replaced all PUD test sets
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/pos_text_types.xlsx
+++ b/data_exploration/acl/tables/pos_text_types.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="75">
   <si>
     <t>Group</t>
   </si>
@@ -207,9 +207,6 @@
     <t>HK</t>
   </si>
   <si>
-    <t>Parliament, Wikipedia, Web</t>
-  </si>
-  <si>
     <t>Movies, Parliament</t>
   </si>
   <si>
@@ -247,6 +244,12 @@
   </si>
   <si>
     <t>NArabizi</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Test Type</t>
   </si>
 </sst>
 </file>
@@ -551,6 +554,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -569,31 +575,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -606,41 +615,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0"/>
-          <bgColor rgb="FFD2E6C4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -944,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,28 +936,20 @@
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -986,14 +959,8 @@
       <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1003,14 +970,8 @@
       <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1020,14 +981,8 @@
       <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1037,14 +992,8 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1054,14 +1003,8 @@
       <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1071,14 +1014,8 @@
       <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1088,65 +1025,41 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>62</v>
       </c>
-      <c r="B11" t="s">
-        <v>63</v>
-      </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1154,16 +1067,10 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1173,14 +1080,8 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1188,16 +1089,10 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1205,16 +1100,10 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1222,16 +1111,10 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1241,14 +1124,8 @@
       <c r="C17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1258,59 +1135,41 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="D18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
         <v>68</v>
       </c>
-      <c r="B19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>69</v>
       </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>71</v>
       </c>
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="21" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="G24:G27">
+  <conditionalFormatting sqref="E24:E27">
     <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
@@ -1340,7 +1199,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G24:G27</xm:sqref>
+          <xm:sqref>E24:E27</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1379,19 +1238,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="25" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -1399,31 +1258,31 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="23"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -1431,11 +1290,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="25"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="26"/>
       <c r="F5" s="7" t="s">
         <v>33</v>
       </c>
@@ -1447,13 +1306,13 @@
       <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -1463,27 +1322,27 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="25"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="23" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="25" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -1491,43 +1350,43 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="31"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="26"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="23"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="23" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="25" t="s">
         <v>27</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -1535,31 +1394,31 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="23"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="25"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -1567,11 +1426,11 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="25"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="7" t="s">
         <v>33</v>
       </c>
@@ -1597,19 +1456,19 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -1617,29 +1476,29 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="25"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -1647,11 +1506,11 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="25"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="7" t="s">
         <v>33</v>
       </c>
@@ -1677,19 +1536,19 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="23" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -1697,31 +1556,31 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="23"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="25"/>
+      <c r="E22" s="26"/>
       <c r="F22" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="23" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F23" s="6" t="s">
@@ -1729,26 +1588,26 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="31"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="35" t="s">
+      <c r="E24" s="31"/>
+      <c r="F24" s="37" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="23"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="16"/>
-      <c r="F25" s="36"/>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -1763,7 +1622,7 @@
       <c r="D26" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -1777,25 +1636,25 @@
       <c r="D27" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="25"/>
+      <c r="E27" s="26"/>
       <c r="F27" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="24" t="s">
+      <c r="D28" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="25" t="s">
         <v>32</v>
       </c>
       <c r="F28" s="6" t="s">
@@ -1803,11 +1662,11 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="25"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="7" t="s">
         <v>33</v>
       </c>
@@ -1834,17 +1693,33 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="E8:E10"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -1855,35 +1730,19 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E26:E27"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A23:A25"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:F13">
     <cfRule type="dataBar" priority="4">

</xml_diff>

<commit_message>
Minor changes to PoS origin
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/pos_text_types.xlsx
+++ b/data_exploration/acl/tables/pos_text_types.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
   <si>
     <t>Group</t>
   </si>
@@ -183,9 +183,6 @@
     <t>AnCora</t>
   </si>
   <si>
-    <t>Fiction, News, Non-fiction</t>
-  </si>
-  <si>
     <t>Norwegian</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>GDT</t>
   </si>
   <si>
-    <t>Europarliament, Wikipedia, Web</t>
-  </si>
-  <si>
     <t>Cantonese</t>
   </si>
   <si>
@@ -249,7 +243,10 @@
     <t>Dataset</t>
   </si>
   <si>
-    <t>Test Type</t>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Parliament, Wikipedia, Web</t>
   </si>
 </sst>
 </file>
@@ -557,64 +554,64 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -928,7 +925,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,10 +940,10 @@
         <v>17</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -979,15 +976,15 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
         <v>53</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -995,13 +992,13 @@
     </row>
     <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1039,21 +1036,21 @@
     </row>
     <row r="10" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -1067,7 +1064,7 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,7 +1086,7 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1100,7 +1097,7 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1111,7 +1108,7 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1138,24 +1135,24 @@
     </row>
     <row r="19" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
         <v>69</v>
-      </c>
-      <c r="B20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1238,19 +1235,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="30" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="23" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -1258,31 +1255,31 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="24"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="26"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -1290,11 +1287,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="26"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="7" t="s">
         <v>33</v>
       </c>
@@ -1306,13 +1303,13 @@
       <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -1322,27 +1319,27 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="26"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="30" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -1350,43 +1347,43 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="27"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="26"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="23" t="s">
         <v>27</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -1394,31 +1391,31 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="26"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -1426,11 +1423,11 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="26"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="7" t="s">
         <v>33</v>
       </c>
@@ -1456,19 +1453,19 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -1476,29 +1473,29 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="26"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -1506,11 +1503,11 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="26"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="7" t="s">
         <v>33</v>
       </c>
@@ -1536,19 +1533,19 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="30" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -1556,31 +1553,31 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="24"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="31"/>
       <c r="D22" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="26"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="30" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F23" s="6" t="s">
@@ -1588,26 +1585,26 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="27"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="37" t="s">
+      <c r="E24" s="25"/>
+      <c r="F24" s="21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="24"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="31"/>
       <c r="D25" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="16"/>
-      <c r="F25" s="38"/>
+      <c r="F25" s="22"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -1622,7 +1619,7 @@
       <c r="D26" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -1636,25 +1633,25 @@
       <c r="D27" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="26"/>
+      <c r="E27" s="24"/>
       <c r="F27" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="25" t="s">
+      <c r="D28" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="23" t="s">
         <v>32</v>
       </c>
       <c r="F28" s="6" t="s">
@@ -1662,11 +1659,11 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="26"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="7" t="s">
         <v>33</v>
       </c>
@@ -1693,6 +1690,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E23:E24"/>
@@ -1709,40 +1740,6 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:F13">
     <cfRule type="dataBar" priority="4">

</xml_diff>